<commit_message>
feat: Initial development of reporter workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\OnboardingReporter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC7C1CB-521E-4C83-9149-19DCB9F9D33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-195" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -159,7 +159,10 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>CandidatesQueue</t>
+  </si>
+  <si>
+    <t>OnboardingEmailCoordinator</t>
   </si>
 </sst>
 </file>
@@ -212,10 +215,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -239,9 +242,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +282,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +388,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -598,7 +601,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
@@ -2782,7 +2787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
generate report starter pack
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\OnboardingReporter\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/bellian_otieno_griffinglobaltech_com/Documents/Documents/UiPath/OnboardingReporter/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC7C1CB-521E-4C83-9149-19DCB9F9D33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{4FC7C1CB-521E-4C83-9149-19DCB9F9D33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCCC7657-1AB4-46A5-9BB7-5FDA918E8B53}"/>
   <bookViews>
-    <workbookView xWindow="-195" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="-15780" windowWidth="21600" windowHeight="11175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>OnboardingEmailCoordinator</t>
+  </si>
+  <si>
+    <t>ReporterSubject</t>
+  </si>
+  <si>
+    <t>Hello, find attached the details of the onboarding Robot Process Automation</t>
+  </si>
+  <si>
+    <t>ReporterBody</t>
+  </si>
+  <si>
+    <t>OnBoarding Bot Report</t>
   </si>
 </sst>
 </file>
@@ -540,16 +552,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -597,7 +609,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -609,7 +621,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1624,16 +1636,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1682,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1681,7 +1693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1795,7 +1807,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1807,8 +1819,22 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2789,12 +2815,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Added SQL queries as assets
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\OnboardingReporter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722931ED-B68C-4741-AA07-8A9398832297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD44F39-224F-4A55-9D86-269915F2EDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-195" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>EmailCredentials</t>
+  </si>
+  <si>
+    <t>GetAverageProcessingTimeQuery</t>
+  </si>
+  <si>
+    <t>GetLongRunningTransactionsQuery</t>
+  </si>
+  <si>
+    <t>GetTransactionStatusAggregatesQuery</t>
+  </si>
+  <si>
+    <t>GetDateRangeQuery</t>
   </si>
 </sst>
 </file>
@@ -2823,7 +2835,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2878,10 +2890,38 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Initial development of the reporter workflow (#3)
* feat: Initial development of reporter workflow

* Refined queries for data retrieval and added detailed annotation

* Implemented error handling

* Improvements...

* Cleaned up workflow, removed unused activities, and renamed variables

* Modified ReFramework for linear execution and transaction handling

* fix: Addressed exception handling issues and performed testing

* Workflow cleanup

* Added SQL queries as assets

* Enhance transaction report with date range and add annotations

* Test new query for separate table

* Refined query to filter transactions by last 7 days
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\OnboardingReporter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD44F39-224F-4A55-9D86-269915F2EDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -159,7 +159,43 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>CandidatesQueue</t>
+  </si>
+  <si>
+    <t>OnboardingEmailCoordinator</t>
+  </si>
+  <si>
+    <t>EmailSubject</t>
+  </si>
+  <si>
+    <t>Automation Error!</t>
+  </si>
+  <si>
+    <t>EmailBody</t>
+  </si>
+  <si>
+    <t>Hello, 
+An exception occurred during the automation process.  Please find the details below:
+Exception Source: @Source
+Exception Message: @Message
+A screenshot of the error has been attached for reference. Please see the attachment for more details.
+Thank you and have a good day,
+Robot :)</t>
+  </si>
+  <si>
+    <t>EmailCredentials</t>
+  </si>
+  <si>
+    <t>GetAverageProcessingTimeQuery</t>
+  </si>
+  <si>
+    <t>GetLongRunningTransactionsQuery</t>
+  </si>
+  <si>
+    <t>GetTransactionStatusAggregatesQuery</t>
+  </si>
+  <si>
+    <t>GetDateRangeQuery</t>
   </si>
 </sst>
 </file>
@@ -212,10 +248,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -239,9 +275,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +315,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +421,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +563,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -538,7 +574,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -598,7 +634,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
@@ -1620,7 +1658,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1802,8 +1840,22 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2782,7 +2834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2828,11 +2882,46 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Minimum Viable Product for generate Reports  (#4)
* feat: Initial development of reporter workflow

* Refined queries for data retrieval and added detailed annotation

* Implemented error handling

* generate report starter pack

* Improvements...

* changes

* unwanted changes

* unwanted changes

* Cleaned up workflow, removed unused activities, and renamed variables

* unwanted changes

* unwanted changes

* Modified ReFramework for linear execution and transaction handling

* fix: Addressed exception handling issues and performed testing

* making progress

* reporter sync

* poor main

* fake process

* fake screenShot

* Minimum viable product

* Workflow cleanup

* Some Changes

* removed unecessary business exceptions

* Added SQL queries as assets

* removed the business exceptions

* Enhance transaction report with date range and add annotations

* good to go

---------

Co-authored-by: Moris Mwai <morismwai1@gmail.com>
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\Documents\UiPath\OnboardingReporter\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/bellian_otieno_griffinglobaltech_com/Documents/Documents/UiPath/OnboardingReporter/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD44F39-224F-4A55-9D86-269915F2EDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{4FC7C1CB-521E-4C83-9149-19DCB9F9D33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B650FA6B-C947-40BE-9E6C-7C9D46C507F1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16470" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -165,6 +165,18 @@
     <t>OnboardingEmailCoordinator</t>
   </si>
   <si>
+    <t>ReporterSubject</t>
+  </si>
+  <si>
+    <t>Hello, find attached the details of the onboarding Robot Process Automation</t>
+  </si>
+  <si>
+    <t>ReporterBody</t>
+  </si>
+  <si>
+    <t>OnBoarding Bot Report</t>
+  </si>
+  <si>
     <t>EmailSubject</t>
   </si>
   <si>
@@ -174,13 +186,7 @@
     <t>EmailBody</t>
   </si>
   <si>
-    <t>Hello, 
-An exception occurred during the automation process.  Please find the details below:
-Exception Source: @Source
-Exception Message: @Message
-A screenshot of the error has been attached for reference. Please see the attachment for more details.
-Thank you and have a good day,
-Robot :)</t>
+    <t xml:space="preserve">Hello, </t>
   </si>
   <si>
     <t>EmailCredentials</t>
@@ -272,6 +278,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,12 +587,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -630,7 +640,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -642,7 +652,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1657,16 +1667,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1703,7 +1713,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1714,7 +1724,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1828,7 +1838,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1842,7 +1852,7 @@
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>
@@ -1850,14 +1860,28 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2832,18 +2856,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2884,42 +2908,42 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>51</v>
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>52</v>
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>53</v>
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>54</v>
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3915,7 +3939,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>